<commit_message>
Whole bunch issues closed
</commit_message>
<xml_diff>
--- a/Gudeline 36 data.xlsx
+++ b/Gudeline 36 data.xlsx
@@ -1,22 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Projects\PsychroCalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBB96C7-215A-4EAE-B9A9-C355550D6A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB99F3F-A889-4C9F-99D5-0A179141360A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Setpoints_Requirements" sheetId="1" r:id="rId1"/>
     <sheet name="Points_Lists" sheetId="2" r:id="rId2"/>
     <sheet name="Sequences" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_Ref38822284" localSheetId="2">Sequences!$A$121</definedName>
+    <definedName name="_Ref440033356" localSheetId="2">Sequences!$B$14</definedName>
+    <definedName name="_Ref73449741" localSheetId="2">Sequences!$A$25</definedName>
+    <definedName name="_Ref73449755" localSheetId="2">Sequences!$A$24</definedName>
+    <definedName name="_Ref73450375" localSheetId="2">Sequences!$A$35</definedName>
+    <definedName name="_Ref73450525" localSheetId="2">Sequences!$A$46</definedName>
+    <definedName name="_Ref73451565" localSheetId="2">Sequences!$A$90</definedName>
+    <definedName name="_Ref73451586" localSheetId="2">Sequences!$A$286</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="171">
   <si>
     <t>Design Requirements Table</t>
   </si>
@@ -529,6 +539,64 @@
   </si>
   <si>
     <t>VAV Terminal Unit</t>
+  </si>
+  <si>
+    <t>Sequence</t>
+  </si>
+  <si>
+    <t>Supply Air Temperature Control</t>
+  </si>
+  <si>
+    <t>Minimum Outdoor Airflow Setpoints</t>
+  </si>
+  <si>
+    <t>Minimum OA Saperate Damper and airflow tracking</t>
+  </si>
+  <si>
+    <t>Minimum OA common Damper and airflow tracking</t>
+  </si>
+  <si>
+    <t>Control of Actuated Relief Dampers without Fans</t>
+  </si>
+  <si>
+    <t>OA Damper</t>
+  </si>
+  <si>
+    <t>Relief fan</t>
+  </si>
+  <si>
+    <t>Relief fan control</t>
+  </si>
+  <si>
+    <t>Building pressure Control</t>
+  </si>
+  <si>
+    <t>Airflow tracking Control</t>
+  </si>
+  <si>
+    <t>Freeze Protection</t>
+  </si>
+  <si>
+    <t>Alarms</t>
+  </si>
+  <si>
+    <t>Automatic Fault Detection and Diagnostics</t>
+  </si>
+  <si>
+    <t>Testing or Commissioning Overrides</t>
+  </si>
+  <si>
+    <t>Plant Requests</t>
+  </si>
+  <si>
+    <t>Supply Fan Control</t>
+  </si>
+  <si>
+    <t>If the supply air temperature drops below 4.4°C (40°F) for 5 minutes, send two (or more, as required to ensure that heating plant is active) heating hot-water plant requests, override the outdoor air damper to the minimum position, and modulate the heating coil to maintain a supply air temperature of at least 6°C (42°F). Disable this function when supply air temperature rises above 7°C (45°F) for 5 minutes.
+If the supply air temperature drops below 3.3°C (38°F) for 5 minutes, fully close both the economizer damper and the minimum outdoor air damper for 1 hour and set a Level 3 alarm noting that minimum ventilation was interrupted. After 1 hour, the unit shall resume minimum outdoor air ventilation and enter the previous stage of freeze protection.
+If it is warm enough that the SAT rises above 7°C (45°F) with minimum ventilation, the unit will remain in Stage 1 freeze protection for 5 minutes then resume normal operation.
+Upon signal from the freeze-stat (if installed), or if supply air temperature drops below 3.3°C (38°F) for 15 minutes or below 1°C (34°F) for 5 minutes, shut down supply and return/relief fan(s), close outdoor air damper, open the cooling-coil valve to 100%, and energize the CHW pump system. Also send two (or more, as required to ensure that heating plant is active) heating hot-water plant requests, modulate the heating coil to maintain the higher of the supply air temperature or the mixed air temperature at 27°C (80°F), and set a Level 2 alarm indicating the unit is shut down by freeze protection.
+If a freeze-protection shutdown is triggered by a low air temperature sensor reading, it shall remain in effect until it is reset by a software switch from the operator’s workstation. (If a freeze-stat with a physical reset switch is used instead, there shall be no software reset switch.)</t>
   </si>
 </sst>
 </file>
@@ -586,7 +654,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -597,11 +665,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="28">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -702,61 +791,73 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{25BABD24-5304-4E68-BF2F-55DFFD748B4E}" name="VAV_and_Reheat_Points" displayName="VAV_and_Reheat_Points" ref="A2:D17" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{25BABD24-5304-4E68-BF2F-55DFFD748B4E}" name="VAV_and_Reheat_Points" displayName="VAV_and_Reheat_Points" ref="A2:D17" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A2:D17" xr:uid="{25BABD24-5304-4E68-BF2F-55DFFD748B4E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D17">
     <sortCondition ref="A2:A17"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{77887A4A-E9CC-404B-A552-7B311ED40798}" name="Required" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{6C7138C9-92BE-4470-AE05-F23E19544C15}" name="Description" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{D5FE7A64-891D-4A48-99A0-FB90811D66E5}" name="Device" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{A1236DED-B651-4A51-BF34-BC1938342E10}" name="Type" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{77887A4A-E9CC-404B-A552-7B311ED40798}" name="Required" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{6C7138C9-92BE-4470-AE05-F23E19544C15}" name="Description" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{D5FE7A64-891D-4A48-99A0-FB90811D66E5}" name="Device" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{A1236DED-B651-4A51-BF34-BC1938342E10}" name="Type" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{ABC6E340-E05C-432A-BC5A-6258665D11DE}" name="Multizone_VAV_Points" displayName="Multizone_VAV_Points" ref="A20:D59" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{ABC6E340-E05C-432A-BC5A-6258665D11DE}" name="Multizone_VAV_Points" displayName="Multizone_VAV_Points" ref="A20:D59" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A20:D59" xr:uid="{ABC6E340-E05C-432A-BC5A-6258665D11DE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:D59">
     <sortCondition ref="A20:A59"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{EDCD7BF4-22AA-445F-B4DD-07C70D201192}" name="Required" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{CE0ECC36-79C9-41C5-BCF0-6672B0795B49}" name="Description" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{A767BE05-76CF-4EDC-ACAE-D2113E87CAAE}" name="Device" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{0FE8A576-664F-4DD5-AB06-3B0FFAE4C8D6}" name="Type" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{EDCD7BF4-22AA-445F-B4DD-07C70D201192}" name="Required" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{CE0ECC36-79C9-41C5-BCF0-6672B0795B49}" name="Description" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{A767BE05-76CF-4EDC-ACAE-D2113E87CAAE}" name="Device" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{0FE8A576-664F-4DD5-AB06-3B0FFAE4C8D6}" name="Type" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A57DA52F-5751-4A35-908D-A7DB01471517}" name="Singlezone_Points" displayName="Singlezone_Points" ref="A62:D98" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A57DA52F-5751-4A35-908D-A7DB01471517}" name="Singlezone_Points" displayName="Singlezone_Points" ref="A62:D98" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A62:D98" xr:uid="{A57DA52F-5751-4A35-908D-A7DB01471517}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A63:D98">
     <sortCondition ref="A62:A98"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5E964800-09EE-4411-9179-5126D316AF9F}" name="Required" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{1452D3F0-E1CE-4555-AC4A-F0EA546235D1}" name="Description" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{1794FB9B-87CC-4796-B633-86087FEB1F2D}" name="Device" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{569B0629-8088-4E40-90F1-2564CBB77CDC}" name="Type" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{5E964800-09EE-4411-9179-5126D316AF9F}" name="Required" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{1452D3F0-E1CE-4555-AC4A-F0EA546235D1}" name="Description" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{1794FB9B-87CC-4796-B633-86087FEB1F2D}" name="Device" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{569B0629-8088-4E40-90F1-2564CBB77CDC}" name="Type" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0941199B-66CB-4A35-92B6-F3297A9F873C}" name="exhaust_fan_points" displayName="exhaust_fan_points" ref="A101:D104" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0941199B-66CB-4A35-92B6-F3297A9F873C}" name="exhaust_fan_points" displayName="exhaust_fan_points" ref="A101:D104" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A101:D104" xr:uid="{0941199B-66CB-4A35-92B6-F3297A9F873C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{18FB9AC0-401D-4730-B7AB-63229E842A4E}" name="Required" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{947677B8-1AD4-4523-A6FE-46A11B740B85}" name="Description" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{6DDD2D7A-A6F8-402C-95CC-9B13B3B3B9A2}" name="Device" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{1A9205DF-BF15-447F-9516-7E6E243993B9}" name="Type" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{18FB9AC0-401D-4730-B7AB-63229E842A4E}" name="Required" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{947677B8-1AD4-4523-A6FE-46A11B740B85}" name="Description" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{6DDD2D7A-A6F8-402C-95CC-9B13B3B3B9A2}" name="Device" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{1A9205DF-BF15-447F-9516-7E6E243993B9}" name="Type" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{627E4CE9-6691-4AFC-859C-E7C0D746D35A}" name="Table6" displayName="Table6" ref="A2:C16" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A2:C16" xr:uid="{627E4CE9-6691-4AFC-859C-E7C0D746D35A}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{8AE4E238-82D6-4B78-B82A-3C0A4C6B2566}" name="Required" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{88D4DF17-A024-4DE7-83C0-C7AC4C1C7FEF}" name="Description" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{16EF8E91-9739-45BA-BC45-CC656357BCAD}" name="Sequence" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1170,8 +1271,8 @@
   </sheetPr>
   <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="113" zoomScaleNormal="151" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView topLeftCell="A22" zoomScale="113" zoomScaleNormal="151" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2593,12 +2694,170 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F29F9F55-D29D-4BAC-AD64-D314BD34B2FA}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="160.6640625" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C16" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>